<commit_message>
Deleted the warning - (Task #455)
---
Task #455: Exported excel contains outdated warning
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.uiengine.ui/resources/TableViewTemplate.xlsx
+++ b/de.dlr.sc.virsat.uiengine.ui/resources/TableViewTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="105" windowWidth="20115" windowHeight="9525"/>
+    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">VirSat IO Sheet </t>
   </si>
   <si>
-    <t>This Document has been generated using Virtual Satellite 4 and belongs to the Virsat Project. Distribution without permission is not allowed!</t>
+    <t>This Document has been generated using Virtual Satellite 4.</t>
   </si>
 </sst>
 </file>
@@ -256,8 +256,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1722120</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>504825</xdr:rowOff>
     </xdr:to>
@@ -283,8 +283,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3695700" y="47625"/>
-          <a:ext cx="2076450" cy="457200"/>
+          <a:off x="3798570" y="47625"/>
+          <a:ext cx="1703070" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -609,17 +609,17 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -658,57 +658,57 @@
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>2</v>
       </c>

</xml_diff>